<commit_message>
Update Dataset Load_Unload Sub-Group members.xlsx
Group members list updated
</commit_message>
<xml_diff>
--- a/Load_Unload_Sub_Group/Dataset Load_Unload Sub-Group members.xlsx
+++ b/Load_Unload_Sub_Group/Dataset Load_Unload Sub-Group members.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OHI\S-101\DCEG\DCEG Sub-Groups\Dataset_Load_Unload_Strategy_Sub_Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmouden\Documents\GitHub\S-101-Documentation-and-FC\Load_Unload_Sub_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB072FF3-9CBB-4B3D-8801-117A56395178}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96287712-02CB-44CC-9DE4-5928BDFE2640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27146" windowHeight="10226" xr2:uid="{986E6AEA-522F-4D19-877D-F9B660639AA5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Australia</t>
   </si>
@@ -167,6 +167,15 @@
       </rPr>
       <t>(Lead)</t>
     </r>
+  </si>
+  <si>
+    <t>IC_ENC</t>
+  </si>
+  <si>
+    <t>Jonathan Pritchard</t>
+  </si>
+  <si>
+    <t>jonathan.pritchard@iictechnologies.com</t>
   </si>
 </sst>
 </file>
@@ -234,14 +243,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -557,34 +567,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00927F4B-E82B-46A5-8F07-CED86F268EAE}">
-  <dimension ref="A2:C16"/>
+  <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="22.3828125" customWidth="1"/>
-    <col min="3" max="3" width="32.07421875" customWidth="1"/>
+    <col min="3" max="3" width="35.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -729,6 +739,17 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -738,8 +759,9 @@
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{F14B42DA-8CA1-4C20-AA34-7BD4798129AD}"/>
     <hyperlink ref="C4:C16" r:id="rId2" display="alvaro.sanchez@defence.gov.au" xr:uid="{53C352AD-DC3B-41C6-B82F-BE472B322D35}"/>
+    <hyperlink ref="C17" r:id="rId3" xr:uid="{63F33463-8174-4D6B-88F8-75236A92A734}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>